<commit_message>
rerranging files, additional feature EDA
</commit_message>
<xml_diff>
--- a/capstone check in notes.xlsx
+++ b/capstone check in notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac2d22d054a0a418/DSI/Projects/Predicting-Loan-Defaults/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16463\OneDrive\DSI\Projects\Predicting-Loan-Defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{A275B3FA-00CF-4FB0-B7D2-180DF6DEC16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8E79457B-1DA9-4684-8525-90C9BCB356E1}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="13920" windowHeight="7580" xr2:uid="{69E45C62-6184-417D-B119-A171E31108C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{69E45C62-6184-417D-B119-A171E31108C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
adding real data dictionary
</commit_message>
<xml_diff>
--- a/capstone check in notes.xlsx
+++ b/capstone check in notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16463\OneDrive\DSI\Projects\Predicting-Loan-Defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A275B3FA-00CF-4FB0-B7D2-180DF6DEC16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8E79457B-1DA9-4684-8525-90C9BCB356E1}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{A275B3FA-00CF-4FB0-B7D2-180DF6DEC16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5DD0BD0F-1435-4EE6-AF6C-4FE2E388F325}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{69E45C62-6184-417D-B119-A171E31108C5}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Define HOW we are measuring?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>which is worse, predicting default when they are not, or predicting if they are NOT defaulting and they default</t>
   </si>
@@ -63,7 +60,13 @@
     <t>Plot the ROC curve, find the top left corners</t>
   </si>
   <si>
-    <t>sensitivity</t>
+    <t>Checkin meeting</t>
+  </si>
+  <si>
+    <t>Define HOW we are measuring? Sensitivity</t>
+  </si>
+  <si>
+    <t>Should we have a full data dictionary in readme on original data? Or post cleanup/dropping columns?</t>
   </si>
 </sst>
 </file>
@@ -415,31 +418,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CB464A-CC88-4C17-8ACF-B1D133B57EF7}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="93.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -449,61 +455,133 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
+      <c r="C5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
+      <c r="C6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
+      <c r="C7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
+      <c r="C8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
+      <c r="C9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
         <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>